<commit_message>
IMPLEMENTAÇÃO SEPARADA E FUNCIONAL DO CÁLCULO DE COMISSÕES POR RECEBIMENTO E INICIO DA IMPLEMENTAÇÃO DE UMA AUDITORIA DOS RECEBIMENTOS EM TABELAS FORMATADAS EM PDF
</commit_message>
<xml_diff>
--- a/dados_entrada/Analise_Comercial_Completa.xlsx
+++ b/dados_entrada/Analise_Comercial_Completa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.rafael\Desktop\PROJETO_COMISSOES_V2\dados_entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B65928-6B3D-48A4-88FB-3B93307B4E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F960CB89-8145-41E1-AD1F-3A543E38BEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Processo</t>
   </si>
@@ -118,12 +118,6 @@
   </si>
   <si>
     <t>Numero NF</t>
-  </si>
-  <si>
-    <t>048341</t>
-  </si>
-  <si>
-    <t>CS-Test</t>
   </si>
   <si>
     <t>Sensor</t>
@@ -478,16 +472,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -589,7 +589,7 @@
         <v>23</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>20</v>
@@ -603,8 +603,8 @@
       <c r="R2" t="s">
         <v>29</v>
       </c>
-      <c r="S2" t="s">
-        <v>31</v>
+      <c r="S2">
+        <v>48341</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -661,8 +661,8 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>32</v>
+      <c r="A4">
+        <v>999997</v>
       </c>
       <c r="B4" s="2">
         <v>45920</v>
@@ -680,19 +680,19 @@
         <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -710,10 +710,10 @@
         <v>24</v>
       </c>
       <c r="Q4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GERAÇÃO DE AUDITORIA EM PDF DAS COMISSÕES POR RECEBIMENTO
</commit_message>
<xml_diff>
--- a/dados_entrada/Analise_Comercial_Completa.xlsx
+++ b/dados_entrada/Analise_Comercial_Completa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.rafael\Desktop\PROJETO_COMISSOES_V2\dados_entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F960CB89-8145-41E1-AD1F-3A543E38BEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3121C2F-1F6D-4617-A094-A7FB7C342D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +589,7 @@
         <v>23</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>20</v>
@@ -645,7 +645,7 @@
         <v>23</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>20</v>

</xml_diff>